<commit_message>
Tiếp tục phát triển code để triển khai các yêu cầu: - Phân quyền user / admin, quản lý đăng nhập - Luồng xử lý MOP - Cài đặt và triển khai database PostgreSQL. - Chia đánh giá rủi ro và đánh giá bàn giao. ...
</commit_message>
<xml_diff>
--- a/backend/templates/server_list_template_v2.xlsx
+++ b/backend/templates/server_list_template_v2.xlsx
@@ -444,8 +444,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
@@ -458,22 +458,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>admin_username</t>
+          <t>ssh_username</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>admin_password</t>
+          <t>ssh_password</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>root_username</t>
+          <t>sudo_username</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>root_password</t>
+          <t>sudo_password</t>
         </is>
       </c>
     </row>

</xml_diff>